<commit_message>
updated db...running into issues
</commit_message>
<xml_diff>
--- a/DB/floor1WP.xlsx
+++ b/DB/floor1WP.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="165" windowWidth="13395" windowHeight="11760" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="225" windowWidth="13395" windowHeight="11700" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="node" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="84">
   <si>
     <t>nID</t>
   </si>
@@ -617,15 +617,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE50"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:K50"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="1.28515625" style="1" customWidth="1"/>
     <col min="10" max="18" width="9.85546875" customWidth="1"/>
@@ -714,7 +714,7 @@
         <v>53</v>
       </c>
       <c r="X2" t="str">
-        <f>$B2</f>
+        <f t="shared" ref="X2:X33" si="0">$B2</f>
         <v>f1-100s3</v>
       </c>
       <c r="Y2" t="str">
@@ -722,7 +722,7 @@
         <v>f1-100C1_1</v>
       </c>
       <c r="Z2" t="str">
-        <f>$B2</f>
+        <f t="shared" ref="Z2:Z33" si="1">$B2</f>
         <v>f1-100s3</v>
       </c>
       <c r="AA2">
@@ -730,7 +730,7 @@
         <v>0</v>
       </c>
       <c r="AB2" t="str">
-        <f t="shared" ref="AB2:AD2" si="0">$B2</f>
+        <f t="shared" ref="AB2:AD2" si="2">$B2</f>
         <v>f1-100s3</v>
       </c>
       <c r="AC2">
@@ -738,7 +738,7 @@
         <v>0</v>
       </c>
       <c r="AD2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>f1-100s3</v>
       </c>
       <c r="AE2">
@@ -772,42 +772,42 @@
         <v>2</v>
       </c>
       <c r="K3" t="str">
-        <f t="shared" ref="K3:K50" si="1">J$1 &amp; A3 &amp; ", '" &amp; B3 &amp; "', " &amp; C3 &amp; ", " &amp; D3 &amp; ", " &amp; E3 &amp; ", '" &amp; F3 &amp; "', '" &amp; G3 &amp; "');"</f>
+        <f t="shared" ref="K3:K50" si="3">J$1 &amp; A3 &amp; ", '" &amp; B3 &amp; "', " &amp; C3 &amp; ", " &amp; D3 &amp; ", " &amp; E3 &amp; ", '" &amp; F3 &amp; "', '" &amp; G3 &amp; "');"</f>
         <v>INSERT INTO tblNode VALUES (2, 'f1-nel', 670, 546, 1, 'Elevator', 'Walk-In Clinic');</v>
       </c>
       <c r="S3" t="s">
         <v>54</v>
       </c>
       <c r="X3" t="str">
-        <f>$B3</f>
+        <f t="shared" si="0"/>
         <v>f1-nel</v>
       </c>
       <c r="Y3" t="str">
-        <f t="shared" ref="Y3:Y50" si="2">S3</f>
+        <f t="shared" ref="Y3:Y50" si="4">S3</f>
         <v>f1-100C1_0</v>
       </c>
       <c r="Z3" t="str">
-        <f>$B3</f>
+        <f t="shared" si="1"/>
         <v>f1-nel</v>
       </c>
       <c r="AA3">
-        <f t="shared" ref="AA3:AA50" si="3">T3</f>
+        <f t="shared" ref="AA3:AA50" si="5">T3</f>
         <v>0</v>
       </c>
       <c r="AB3" t="str">
-        <f>$B3</f>
+        <f t="shared" ref="AB3:AB50" si="6">$B3</f>
         <v>f1-nel</v>
       </c>
       <c r="AC3">
-        <f t="shared" ref="AC3:AC50" si="4">U3</f>
+        <f t="shared" ref="AC3:AC50" si="7">U3</f>
         <v>0</v>
       </c>
       <c r="AD3" t="str">
-        <f>$B3</f>
+        <f t="shared" ref="AD3:AD50" si="8">$B3</f>
         <v>f1-nel</v>
       </c>
       <c r="AE3">
-        <f t="shared" ref="AE3:AE50" si="5">V3</f>
+        <f t="shared" ref="AE3:AE50" si="9">V3</f>
         <v>0</v>
       </c>
     </row>
@@ -837,7 +837,7 @@
         <v>4</v>
       </c>
       <c r="K4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO tblNode VALUES (3, 'f1-100C1_0', 697, 464, 1, 'WP', 'Walk-In Clinic');</v>
       </c>
       <c r="S4" t="s">
@@ -847,35 +847,35 @@
         <v>60</v>
       </c>
       <c r="X4" t="str">
-        <f>$B4</f>
+        <f t="shared" si="0"/>
         <v>f1-100C1_0</v>
       </c>
       <c r="Y4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>f1-100C1_1</v>
       </c>
       <c r="Z4" t="str">
-        <f>$B4</f>
+        <f t="shared" si="1"/>
         <v>f1-100C1_0</v>
       </c>
       <c r="AA4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AB4" t="str">
-        <f>$B4</f>
+        <f t="shared" si="6"/>
         <v>f1-100C1_0</v>
       </c>
       <c r="AC4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>f1-nel</v>
       </c>
       <c r="AD4" t="str">
-        <f>$B4</f>
+        <f t="shared" si="8"/>
         <v>f1-100C1_0</v>
       </c>
       <c r="AE4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -905,7 +905,7 @@
         <v>4</v>
       </c>
       <c r="K5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO tblNode VALUES (4, 'f1-100C1_1', 492, 421, 1, 'WP', 'Walk-In Clinic');</v>
       </c>
       <c r="S5" t="s">
@@ -918,35 +918,35 @@
         <v>76</v>
       </c>
       <c r="X5" t="str">
-        <f>$B5</f>
+        <f t="shared" si="0"/>
         <v>f1-100C1_1</v>
       </c>
       <c r="Y5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>f1-100C1_0</v>
       </c>
       <c r="Z5" t="str">
-        <f>$B5</f>
+        <f t="shared" si="1"/>
         <v>f1-100C1_1</v>
       </c>
       <c r="AA5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>f1-100C1_2</v>
       </c>
       <c r="AB5" t="str">
-        <f>$B5</f>
+        <f t="shared" si="6"/>
         <v>f1-100C1_1</v>
       </c>
       <c r="AC5" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>f1-100s3</v>
       </c>
       <c r="AD5" t="str">
-        <f>$B5</f>
+        <f t="shared" si="8"/>
         <v>f1-100C1_1</v>
       </c>
       <c r="AE5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -976,7 +976,7 @@
         <v>4</v>
       </c>
       <c r="K6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO tblNode VALUES (5, 'f1-100C1_2', 359, 394, 1, 'WP', 'Walk-In Clinic');</v>
       </c>
       <c r="S6" t="s">
@@ -986,35 +986,35 @@
         <v>56</v>
       </c>
       <c r="X6" t="str">
-        <f>$B6</f>
+        <f t="shared" si="0"/>
         <v>f1-100C1_2</v>
       </c>
       <c r="Y6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>f1-100C1_1</v>
       </c>
       <c r="Z6" t="str">
-        <f>$B6</f>
+        <f t="shared" si="1"/>
         <v>f1-100C1_2</v>
       </c>
       <c r="AA6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>f1-100C1_3</v>
       </c>
       <c r="AB6" t="str">
-        <f>$B6</f>
+        <f t="shared" si="6"/>
         <v>f1-100C1_2</v>
       </c>
       <c r="AC6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AD6" t="str">
-        <f>$B6</f>
+        <f t="shared" si="8"/>
         <v>f1-100C1_2</v>
       </c>
       <c r="AE6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -1044,7 +1044,7 @@
         <v>4</v>
       </c>
       <c r="K7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO tblNode VALUES (6, 'f1-100C1_3', 255, 909, 1, 'WP', 'Walk-In Clinic');</v>
       </c>
       <c r="S7" t="s">
@@ -1053,36 +1053,39 @@
       <c r="T7" t="s">
         <v>57</v>
       </c>
+      <c r="U7" t="s">
+        <v>45</v>
+      </c>
       <c r="X7" t="str">
-        <f>$B7</f>
+        <f t="shared" si="0"/>
         <v>f1-100C1_3</v>
       </c>
       <c r="Y7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>f1-100C1_2</v>
       </c>
       <c r="Z7" t="str">
-        <f>$B7</f>
+        <f t="shared" si="1"/>
         <v>f1-100C1_3</v>
       </c>
       <c r="AA7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>f1-100C1_4</v>
       </c>
       <c r="AB7" t="str">
-        <f>$B7</f>
+        <f t="shared" si="6"/>
         <v>f1-100C1_3</v>
       </c>
-      <c r="AC7">
-        <f t="shared" si="4"/>
-        <v>0</v>
+      <c r="AC7" t="str">
+        <f t="shared" si="7"/>
+        <v>f1-nr</v>
       </c>
       <c r="AD7" t="str">
-        <f>$B7</f>
+        <f t="shared" si="8"/>
         <v>f1-100C1_3</v>
       </c>
       <c r="AE7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -1112,42 +1115,42 @@
         <v>3</v>
       </c>
       <c r="K8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO tblNode VALUES (7, 'f1-nr', 630, 1289, 1, 'Restroom', 'Walk-In Clinic');</v>
       </c>
       <c r="S8" t="s">
         <v>56</v>
       </c>
       <c r="X8" t="str">
-        <f>$B8</f>
+        <f t="shared" si="0"/>
         <v>f1-nr</v>
       </c>
       <c r="Y8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>f1-100C1_3</v>
       </c>
       <c r="Z8" t="str">
-        <f>$B8</f>
+        <f t="shared" si="1"/>
         <v>f1-nr</v>
       </c>
       <c r="AA8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AB8" t="str">
-        <f>$B8</f>
+        <f t="shared" si="6"/>
         <v>f1-nr</v>
       </c>
       <c r="AC8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AD8" t="str">
-        <f>$B8</f>
+        <f t="shared" si="8"/>
         <v>f1-nr</v>
       </c>
       <c r="AE8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -1177,7 +1180,7 @@
         <v>4</v>
       </c>
       <c r="K9" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO tblNode VALUES (8, 'f1-100C1_4', 1267, 1355, 1, 'WP', 'Walk-In Clinic');</v>
       </c>
       <c r="S9" t="s">
@@ -1187,35 +1190,35 @@
         <v>58</v>
       </c>
       <c r="X9" t="str">
-        <f>$B9</f>
+        <f t="shared" si="0"/>
         <v>f1-100C1_4</v>
       </c>
       <c r="Y9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>f1-100C1_3</v>
       </c>
       <c r="Z9" t="str">
-        <f>$B9</f>
+        <f t="shared" si="1"/>
         <v>f1-100C1_4</v>
       </c>
       <c r="AA9" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>f1-100C1_5</v>
       </c>
       <c r="AB9" t="str">
-        <f>$B9</f>
+        <f t="shared" si="6"/>
         <v>f1-100C1_4</v>
       </c>
       <c r="AC9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AD9" t="str">
-        <f>$B9</f>
+        <f t="shared" si="8"/>
         <v>f1-100C1_4</v>
       </c>
       <c r="AE9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -1245,7 +1248,7 @@
         <v>5</v>
       </c>
       <c r="K10" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO tblNode VALUES (9, 'f1-100C1_5', 1267, 2759, 1, 'WP', 'Walk-In Clinic');</v>
       </c>
       <c r="S10" t="s">
@@ -1258,35 +1261,35 @@
         <v>51</v>
       </c>
       <c r="X10" t="str">
-        <f>$B10</f>
+        <f t="shared" si="0"/>
         <v>f1-100C1_5</v>
       </c>
       <c r="Y10" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>f1-100C1_4</v>
       </c>
       <c r="Z10" t="str">
-        <f>$B10</f>
+        <f t="shared" si="1"/>
         <v>f1-100C1_5</v>
       </c>
       <c r="AA10" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>f1-100C2_0</v>
       </c>
       <c r="AB10" t="str">
-        <f>$B10</f>
+        <f t="shared" si="6"/>
         <v>f1-100C1_5</v>
       </c>
       <c r="AC10" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>f1-108</v>
       </c>
       <c r="AD10" t="str">
-        <f>$B10</f>
+        <f t="shared" si="8"/>
         <v>f1-100C1_5</v>
       </c>
       <c r="AE10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -1316,7 +1319,7 @@
         <v>5</v>
       </c>
       <c r="K11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO tblNode VALUES (10, 'f1-100C2_0', 1267, 3689, 1, 'WP', 'Walk-In Clinic');</v>
       </c>
       <c r="S11" t="s">
@@ -1329,35 +1332,35 @@
         <v>59</v>
       </c>
       <c r="X11" t="str">
-        <f>$B11</f>
+        <f t="shared" si="0"/>
         <v>f1-100C2_0</v>
       </c>
       <c r="Y11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>f1-100C1_5</v>
       </c>
       <c r="Z11" t="str">
-        <f>$B11</f>
+        <f t="shared" si="1"/>
         <v>f1-100C2_0</v>
       </c>
       <c r="AA11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>f1-100C3_0</v>
       </c>
       <c r="AB11" t="str">
-        <f>$B11</f>
+        <f t="shared" si="6"/>
         <v>f1-100C2_0</v>
       </c>
       <c r="AC11" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>f1-sel</v>
       </c>
       <c r="AD11" t="str">
-        <f>$B11</f>
+        <f t="shared" si="8"/>
         <v>f1-100C2_0</v>
       </c>
       <c r="AE11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -1387,42 +1390,45 @@
         <v>5</v>
       </c>
       <c r="K12" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO tblNode VALUES (11, 'f1-100C3_0', 1165, 4093, 1, 'WP', 'Walk-In Clinic');</v>
       </c>
       <c r="S12" t="s">
         <v>62</v>
       </c>
+      <c r="T12" t="s">
+        <v>63</v>
+      </c>
       <c r="X12" t="str">
-        <f>$B12</f>
+        <f t="shared" si="0"/>
         <v>f1-100C3_0</v>
       </c>
       <c r="Y12" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>f1-100C2_0</v>
       </c>
       <c r="Z12" t="str">
-        <f>$B12</f>
+        <f t="shared" si="1"/>
         <v>f1-100C3_0</v>
       </c>
-      <c r="AA12">
-        <f t="shared" si="3"/>
-        <v>0</v>
+      <c r="AA12" t="str">
+        <f t="shared" si="5"/>
+        <v>f1-100C3_1</v>
       </c>
       <c r="AB12" t="str">
-        <f>$B12</f>
+        <f t="shared" si="6"/>
         <v>f1-100C3_0</v>
       </c>
       <c r="AC12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AD12" t="str">
-        <f>$B12</f>
+        <f t="shared" si="8"/>
         <v>f1-100C3_0</v>
       </c>
       <c r="AE12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -1452,7 +1458,7 @@
         <v>5</v>
       </c>
       <c r="K13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO tblNode VALUES (12, 'f1-100C3_1', 1165, 4195, 1, 'WP', 'Walk-In Clinic');</v>
       </c>
       <c r="S13" t="s">
@@ -1462,35 +1468,35 @@
         <v>61</v>
       </c>
       <c r="X13" t="str">
-        <f>$B13</f>
+        <f t="shared" si="0"/>
         <v>f1-100C3_1</v>
       </c>
       <c r="Y13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>f1-100C3_0</v>
       </c>
       <c r="Z13" t="str">
-        <f>$B13</f>
+        <f t="shared" si="1"/>
         <v>f1-100C3_1</v>
       </c>
-      <c r="AA13">
-        <f t="shared" si="3"/>
-        <v>0</v>
+      <c r="AA13" t="str">
+        <f>T12</f>
+        <v>f1-100C3_1</v>
       </c>
       <c r="AB13" t="str">
-        <f>$B13</f>
+        <f t="shared" si="6"/>
         <v>f1-100C3_1</v>
       </c>
       <c r="AC13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>f1-100s2</v>
       </c>
       <c r="AD13" t="str">
-        <f>$B13</f>
+        <f t="shared" si="8"/>
         <v>f1-100C3_1</v>
       </c>
       <c r="AE13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -1520,42 +1526,42 @@
         <v>6</v>
       </c>
       <c r="K14" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO tblNode VALUES (13, 'f1-sel', 460, 3689, 1, 'Elevator', 'Walk-In Clinic');</v>
       </c>
       <c r="S14" t="s">
         <v>62</v>
       </c>
       <c r="X14" t="str">
-        <f>$B14</f>
+        <f t="shared" si="0"/>
         <v>f1-sel</v>
       </c>
       <c r="Y14" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>f1-100C2_0</v>
       </c>
       <c r="Z14" t="str">
-        <f>$B14</f>
+        <f t="shared" si="1"/>
         <v>f1-sel</v>
       </c>
       <c r="AA14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AB14" t="str">
-        <f>$B14</f>
+        <f t="shared" si="6"/>
         <v>f1-sel</v>
       </c>
       <c r="AC14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AD14" t="str">
-        <f>$B14</f>
+        <f t="shared" si="8"/>
         <v>f1-sel</v>
       </c>
       <c r="AE14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -1585,42 +1591,42 @@
         <v>7</v>
       </c>
       <c r="K15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO tblNode VALUES (14, 'f1-100s2', 936, 4195, 1, 'Stair', 'Walk-In Clinic');</v>
       </c>
       <c r="S15" t="s">
         <v>63</v>
       </c>
       <c r="X15" t="str">
-        <f>$B15</f>
+        <f t="shared" si="0"/>
         <v>f1-100s2</v>
       </c>
       <c r="Y15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>f1-100C3_1</v>
       </c>
       <c r="Z15" t="str">
-        <f>$B15</f>
+        <f t="shared" si="1"/>
         <v>f1-100s2</v>
       </c>
       <c r="AA15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AB15" t="str">
-        <f>$B15</f>
+        <f t="shared" si="6"/>
         <v>f1-100s2</v>
       </c>
       <c r="AC15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AD15" t="str">
-        <f>$B15</f>
+        <f t="shared" si="8"/>
         <v>f1-100s2</v>
       </c>
       <c r="AE15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -1650,7 +1656,7 @@
         <v>16</v>
       </c>
       <c r="K16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO tblNode VALUES (15, 'f1-108', 1101, 2759, 1, 'Entrance', 'Walk-In Clinic');</v>
       </c>
       <c r="S16" t="s">
@@ -1660,35 +1666,35 @@
         <v>13</v>
       </c>
       <c r="X16" t="str">
-        <f>$B16</f>
+        <f t="shared" si="0"/>
         <v>f1-108</v>
       </c>
       <c r="Y16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>f1-100C1_5</v>
       </c>
       <c r="Z16" t="str">
-        <f>$B16</f>
+        <f t="shared" si="1"/>
         <v>f1-108</v>
       </c>
       <c r="AA16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>f1-108_0</v>
       </c>
       <c r="AB16" t="str">
-        <f>$B16</f>
+        <f t="shared" si="6"/>
         <v>f1-108</v>
       </c>
       <c r="AC16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AD16" t="str">
-        <f>$B16</f>
+        <f t="shared" si="8"/>
         <v>f1-108</v>
       </c>
       <c r="AE16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -1718,7 +1724,7 @@
         <v>17</v>
       </c>
       <c r="K17" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO tblNode VALUES (16, 'f1-108_0', 905, 2759, 1, 'Reception', 'Walk-In Clinic');</v>
       </c>
       <c r="S17" t="s">
@@ -1728,35 +1734,35 @@
         <v>14</v>
       </c>
       <c r="X17" t="str">
-        <f>$B17</f>
+        <f t="shared" si="0"/>
         <v>f1-108_0</v>
       </c>
       <c r="Y17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>f1-108</v>
       </c>
       <c r="Z17" t="str">
-        <f>$B17</f>
+        <f t="shared" si="1"/>
         <v>f1-108_0</v>
       </c>
       <c r="AA17" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>f1-108_1</v>
       </c>
       <c r="AB17" t="str">
-        <f>$B17</f>
+        <f t="shared" si="6"/>
         <v>f1-108_0</v>
       </c>
       <c r="AC17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AD17" t="str">
-        <f>$B17</f>
+        <f t="shared" si="8"/>
         <v>f1-108_0</v>
       </c>
       <c r="AE17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -1786,7 +1792,7 @@
         <v>18</v>
       </c>
       <c r="K18" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO tblNode VALUES (17, 'f1-108_1', 905, 2939, 1, 'WP', 'Walk-In Clinic');</v>
       </c>
       <c r="S18" t="s">
@@ -1796,35 +1802,35 @@
         <v>15</v>
       </c>
       <c r="X18" t="str">
-        <f>$B18</f>
+        <f t="shared" si="0"/>
         <v>f1-108_1</v>
       </c>
       <c r="Y18" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>f1-108_0</v>
       </c>
       <c r="Z18" t="str">
-        <f>$B18</f>
+        <f t="shared" si="1"/>
         <v>f1-108_1</v>
       </c>
       <c r="AA18" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>f1-108_2</v>
       </c>
       <c r="AB18" t="str">
-        <f>$B18</f>
+        <f t="shared" si="6"/>
         <v>f1-108_1</v>
       </c>
       <c r="AC18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AD18" t="str">
-        <f>$B18</f>
+        <f t="shared" si="8"/>
         <v>f1-108_1</v>
       </c>
       <c r="AE18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -1854,7 +1860,7 @@
         <v>18</v>
       </c>
       <c r="K19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO tblNode VALUES (18, 'f1-108_2', 646, 2939, 1, 'WP', 'Walk-In Clinic');</v>
       </c>
       <c r="S19" t="s">
@@ -1864,35 +1870,35 @@
         <v>14</v>
       </c>
       <c r="X19" t="str">
-        <f>$B19</f>
+        <f t="shared" si="0"/>
         <v>f1-108_2</v>
       </c>
       <c r="Y19" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>f1-108A1</v>
       </c>
       <c r="Z19" t="str">
-        <f>$B19</f>
+        <f t="shared" si="1"/>
         <v>f1-108_2</v>
       </c>
       <c r="AA19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>f1-108_1</v>
       </c>
       <c r="AB19" t="str">
-        <f>$B19</f>
+        <f t="shared" si="6"/>
         <v>f1-108_2</v>
       </c>
       <c r="AC19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AD19" t="str">
-        <f>$B19</f>
+        <f t="shared" si="8"/>
         <v>f1-108_2</v>
       </c>
       <c r="AE19">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -1922,7 +1928,7 @@
         <v>19</v>
       </c>
       <c r="K20" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO tblNode VALUES (19, 'f1-108A1', 646, 2828, 1, 'Entrance', 'Walk-In Clinic');</v>
       </c>
       <c r="S20" t="s">
@@ -1932,35 +1938,35 @@
         <v>15</v>
       </c>
       <c r="X20" t="str">
-        <f>$B20</f>
+        <f t="shared" si="0"/>
         <v>f1-108A1</v>
       </c>
       <c r="Y20" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>f1-108A1_0</v>
       </c>
       <c r="Z20" t="str">
-        <f>$B20</f>
+        <f t="shared" si="1"/>
         <v>f1-108A1</v>
       </c>
       <c r="AA20" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>f1-108_2</v>
       </c>
       <c r="AB20" t="str">
-        <f>$B20</f>
+        <f t="shared" si="6"/>
         <v>f1-108A1</v>
       </c>
       <c r="AC20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AD20" t="str">
-        <f>$B20</f>
+        <f t="shared" si="8"/>
         <v>f1-108A1</v>
       </c>
       <c r="AE20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -1990,7 +1996,7 @@
         <v>74</v>
       </c>
       <c r="K21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO tblNode VALUES (20, 'f1-108A1_0', 646, 2738, 1, 'WP', 'Walk-In Clinic');</v>
       </c>
       <c r="S21" t="s">
@@ -2003,35 +2009,35 @@
         <v>48</v>
       </c>
       <c r="X21" t="str">
-        <f>$B21</f>
+        <f t="shared" si="0"/>
         <v>f1-108A1_0</v>
       </c>
       <c r="Y21" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>f1-108A1</v>
       </c>
       <c r="Z21" t="str">
-        <f>$B21</f>
+        <f t="shared" si="1"/>
         <v>f1-108A1_0</v>
       </c>
       <c r="AA21" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>f1-108A1_1</v>
       </c>
       <c r="AB21" t="str">
-        <f>$B21</f>
+        <f t="shared" si="6"/>
         <v>f1-108A1_0</v>
       </c>
       <c r="AC21" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>f1-108P</v>
       </c>
       <c r="AD21" t="str">
-        <f>$B21</f>
+        <f t="shared" si="8"/>
         <v>f1-108A1_0</v>
       </c>
       <c r="AE21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -2061,7 +2067,7 @@
         <v>74</v>
       </c>
       <c r="K22" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO tblNode VALUES (21, 'f1-108A1_1', 646, 2634, 1, 'WP', 'Walk-In Clinic');</v>
       </c>
       <c r="S22" t="s">
@@ -2074,35 +2080,35 @@
         <v>22</v>
       </c>
       <c r="X22" t="str">
-        <f>$B22</f>
+        <f t="shared" si="0"/>
         <v>f1-108A1_1</v>
       </c>
       <c r="Y22" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>f1-108A1_0</v>
       </c>
       <c r="Z22" t="str">
-        <f>$B22</f>
+        <f t="shared" si="1"/>
         <v>f1-108A1_1</v>
       </c>
       <c r="AA22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>f1-108A1_2</v>
       </c>
       <c r="AB22" t="str">
-        <f>$B22</f>
+        <f t="shared" si="6"/>
         <v>f1-108A1_1</v>
       </c>
       <c r="AC22" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>f1-108B</v>
       </c>
       <c r="AD22" t="str">
-        <f>$B22</f>
+        <f t="shared" si="8"/>
         <v>f1-108A1_1</v>
       </c>
       <c r="AE22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -2132,7 +2138,7 @@
         <v>74</v>
       </c>
       <c r="K23" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO tblNode VALUES (22, 'f1-108A1_2', 646, 2558, 1, 'WP', 'Walk-In Clinic');</v>
       </c>
       <c r="S23" t="s">
@@ -2145,35 +2151,35 @@
         <v>47</v>
       </c>
       <c r="X23" t="str">
-        <f>$B23</f>
+        <f t="shared" si="0"/>
         <v>f1-108A1_2</v>
       </c>
       <c r="Y23" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>f1-108A1_1</v>
       </c>
       <c r="Z23" t="str">
-        <f>$B23</f>
+        <f t="shared" si="1"/>
         <v>f1-108A1_2</v>
       </c>
       <c r="AA23" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>f1-108A1_3</v>
       </c>
       <c r="AB23" t="str">
-        <f>$B23</f>
+        <f t="shared" si="6"/>
         <v>f1-108A1_2</v>
       </c>
       <c r="AC23" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>f1-108O</v>
       </c>
       <c r="AD23" t="str">
-        <f>$B23</f>
+        <f t="shared" si="8"/>
         <v>f1-108A1_2</v>
       </c>
       <c r="AE23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -2203,7 +2209,7 @@
         <v>74</v>
       </c>
       <c r="K24" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO tblNode VALUES (23, 'f1-108A1_3', 646, 2519, 1, 'WP', 'Walk-In Clinic');</v>
       </c>
       <c r="S24" t="s">
@@ -2216,35 +2222,35 @@
         <v>23</v>
       </c>
       <c r="X24" t="str">
-        <f>$B24</f>
+        <f t="shared" si="0"/>
         <v>f1-108A1_3</v>
       </c>
       <c r="Y24" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>f1-108A1_2</v>
       </c>
       <c r="Z24" t="str">
-        <f>$B24</f>
+        <f t="shared" si="1"/>
         <v>f1-108A1_3</v>
       </c>
       <c r="AA24" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>f1-108A1_4</v>
       </c>
       <c r="AB24" t="str">
-        <f>$B24</f>
+        <f t="shared" si="6"/>
         <v>f1-108A1_3</v>
       </c>
       <c r="AC24" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>f1-108C</v>
       </c>
       <c r="AD24" t="str">
-        <f>$B24</f>
+        <f t="shared" si="8"/>
         <v>f1-108A1_3</v>
       </c>
       <c r="AE24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -2274,7 +2280,7 @@
         <v>74</v>
       </c>
       <c r="K25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO tblNode VALUES (24, 'f1-108A1_4', 646, 2477, 1, 'WP', 'Walk-In Clinic');</v>
       </c>
       <c r="S25" t="s">
@@ -2287,35 +2293,35 @@
         <v>65</v>
       </c>
       <c r="X25" t="str">
-        <f>$B25</f>
+        <f t="shared" si="0"/>
         <v>f1-108A1_4</v>
       </c>
       <c r="Y25" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>f1-108A1_3</v>
       </c>
       <c r="Z25" t="str">
-        <f>$B25</f>
+        <f t="shared" si="1"/>
         <v>f1-108A1_4</v>
       </c>
       <c r="AA25" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>f1-108A1_5</v>
       </c>
       <c r="AB25" t="str">
-        <f>$B25</f>
+        <f t="shared" si="6"/>
         <v>f1-108A1_4</v>
       </c>
       <c r="AC25" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>f1-108T1</v>
       </c>
       <c r="AD25" t="str">
-        <f>$B25</f>
+        <f t="shared" si="8"/>
         <v>f1-108A1_4</v>
       </c>
       <c r="AE25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -2345,7 +2351,7 @@
         <v>74</v>
       </c>
       <c r="K26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO tblNode VALUES (25, 'f1-108A1_5', 646, 2360, 1, 'WP', 'Walk-In Clinic');</v>
       </c>
       <c r="S26" t="s">
@@ -2358,35 +2364,35 @@
         <v>24</v>
       </c>
       <c r="X26" t="str">
-        <f>$B26</f>
+        <f t="shared" si="0"/>
         <v>f1-108A1_5</v>
       </c>
       <c r="Y26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>f1-108A1_4</v>
       </c>
       <c r="Z26" t="str">
-        <f>$B26</f>
+        <f t="shared" si="1"/>
         <v>f1-108A1_5</v>
       </c>
       <c r="AA26" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>f1-108A1_6</v>
       </c>
       <c r="AB26" t="str">
-        <f>$B26</f>
+        <f t="shared" si="6"/>
         <v>f1-108A1_5</v>
       </c>
       <c r="AC26" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>f1-108D</v>
       </c>
       <c r="AD26" t="str">
-        <f>$B26</f>
+        <f t="shared" si="8"/>
         <v>f1-108A1_5</v>
       </c>
       <c r="AE26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -2416,7 +2422,7 @@
         <v>74</v>
       </c>
       <c r="K27" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO tblNode VALUES (26, 'f1-108A1_6', 646, 2281, 1, 'WP', 'Walk-In Clinic');</v>
       </c>
       <c r="S27" t="s">
@@ -2429,35 +2435,35 @@
         <v>66</v>
       </c>
       <c r="X27" t="str">
-        <f>$B27</f>
+        <f t="shared" si="0"/>
         <v>f1-108A1_6</v>
       </c>
       <c r="Y27" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>f1-108A1_5</v>
       </c>
       <c r="Z27" t="str">
-        <f>$B27</f>
+        <f t="shared" si="1"/>
         <v>f1-108A1_6</v>
       </c>
       <c r="AA27" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>f1-108A1_7</v>
       </c>
       <c r="AB27" t="str">
-        <f>$B27</f>
+        <f t="shared" si="6"/>
         <v>f1-108A1_6</v>
       </c>
       <c r="AC27" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>f1-108T2</v>
       </c>
       <c r="AD27" t="str">
-        <f>$B27</f>
+        <f t="shared" si="8"/>
         <v>f1-108A1_6</v>
       </c>
       <c r="AE27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -2487,7 +2493,7 @@
         <v>74</v>
       </c>
       <c r="K28" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO tblNode VALUES (27, 'f1-108A1_7', 646, 2235, 1, 'WP', 'Walk-In Clinic');</v>
       </c>
       <c r="S28" t="s">
@@ -2500,35 +2506,35 @@
         <v>25</v>
       </c>
       <c r="X28" t="str">
-        <f>$B28</f>
+        <f t="shared" si="0"/>
         <v>f1-108A1_7</v>
       </c>
       <c r="Y28" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>f1-108A1_6</v>
       </c>
       <c r="Z28" t="str">
-        <f>$B28</f>
+        <f t="shared" si="1"/>
         <v>f1-108A1_7</v>
       </c>
       <c r="AA28" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>f1-108A1_8</v>
       </c>
       <c r="AB28" t="str">
-        <f>$B28</f>
+        <f t="shared" si="6"/>
         <v>f1-108A1_7</v>
       </c>
       <c r="AC28" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>f1-108E</v>
       </c>
       <c r="AD28" t="str">
-        <f>$B28</f>
+        <f t="shared" si="8"/>
         <v>f1-108A1_7</v>
       </c>
       <c r="AE28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -2558,7 +2564,7 @@
         <v>74</v>
       </c>
       <c r="K29" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO tblNode VALUES (28, 'f1-108A1_8', 646, 2220, 1, 'WP', 'Walk-In Clinic');</v>
       </c>
       <c r="S29" t="s">
@@ -2571,35 +2577,35 @@
         <v>46</v>
       </c>
       <c r="X29" t="str">
-        <f>$B29</f>
+        <f t="shared" si="0"/>
         <v>f1-108A1_8</v>
       </c>
       <c r="Y29" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>f1-108A1_7</v>
       </c>
       <c r="Z29" t="str">
-        <f>$B29</f>
+        <f t="shared" si="1"/>
         <v>f1-108A1_8</v>
       </c>
       <c r="AA29" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>f1-108A1_9</v>
       </c>
       <c r="AB29" t="str">
-        <f>$B29</f>
+        <f t="shared" si="6"/>
         <v>f1-108A1_8</v>
       </c>
       <c r="AC29" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>f1-108L</v>
       </c>
       <c r="AD29" t="str">
-        <f>$B29</f>
+        <f t="shared" si="8"/>
         <v>f1-108A1_8</v>
       </c>
       <c r="AE29">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -2629,7 +2635,7 @@
         <v>74</v>
       </c>
       <c r="K30" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO tblNode VALUES (29, 'f1-108A1_9', 646, 2145, 1, 'WP', 'Walk-In Clinic');</v>
       </c>
       <c r="S30" t="s">
@@ -2642,35 +2648,35 @@
         <v>26</v>
       </c>
       <c r="X30" t="str">
-        <f>$B30</f>
+        <f t="shared" si="0"/>
         <v>f1-108A1_9</v>
       </c>
       <c r="Y30" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>f1-108A1_8</v>
       </c>
       <c r="Z30" t="str">
-        <f>$B30</f>
+        <f t="shared" si="1"/>
         <v>f1-108A1_9</v>
       </c>
       <c r="AA30" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>f1-108A1_10</v>
       </c>
       <c r="AB30" t="str">
-        <f>$B30</f>
+        <f t="shared" si="6"/>
         <v>f1-108A1_9</v>
       </c>
       <c r="AC30" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>f1-108F</v>
       </c>
       <c r="AD30" t="str">
-        <f>$B30</f>
+        <f t="shared" si="8"/>
         <v>f1-108A1_9</v>
       </c>
       <c r="AE30">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -2700,7 +2706,7 @@
         <v>74</v>
       </c>
       <c r="K31" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO tblNode VALUES (30, 'f1-108A1_10', 646, 2100, 1, 'WP', 'Walk-In Clinic');</v>
       </c>
       <c r="S31" t="s">
@@ -2713,35 +2719,35 @@
         <v>31</v>
       </c>
       <c r="X31" t="str">
-        <f>$B31</f>
+        <f t="shared" si="0"/>
         <v>f1-108A1_10</v>
       </c>
       <c r="Y31" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>f1-108A1_9</v>
       </c>
       <c r="Z31" t="str">
-        <f>$B31</f>
+        <f t="shared" si="1"/>
         <v>f1-108A1_10</v>
       </c>
       <c r="AA31" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>f1-108A1_11</v>
       </c>
       <c r="AB31" t="str">
-        <f>$B31</f>
+        <f t="shared" si="6"/>
         <v>f1-108A1_10</v>
       </c>
       <c r="AC31" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>f1-108K</v>
       </c>
       <c r="AD31" t="str">
-        <f>$B31</f>
+        <f t="shared" si="8"/>
         <v>f1-108A1_10</v>
       </c>
       <c r="AE31">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -2771,7 +2777,7 @@
         <v>74</v>
       </c>
       <c r="K32" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO tblNode VALUES (31, 'f1-108A1_11', 646, 1986, 1, 'WP', 'Walk-In Clinic');</v>
       </c>
       <c r="S32" t="s">
@@ -2787,35 +2793,35 @@
         <v>27</v>
       </c>
       <c r="X32" t="str">
-        <f>$B32</f>
+        <f t="shared" si="0"/>
         <v>f1-108A1_11</v>
       </c>
       <c r="Y32" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>f1-108A1_10</v>
       </c>
       <c r="Z32" t="str">
-        <f>$B32</f>
+        <f t="shared" si="1"/>
         <v>f1-108A1_11</v>
       </c>
       <c r="AA32" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>f1-108A1_12</v>
       </c>
       <c r="AB32" t="str">
-        <f>$B32</f>
+        <f t="shared" si="6"/>
         <v>f1-108A1_11</v>
       </c>
       <c r="AC32" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>f1-108J</v>
       </c>
       <c r="AD32" t="str">
-        <f>$B32</f>
+        <f t="shared" si="8"/>
         <v>f1-108A1_11</v>
       </c>
       <c r="AE32" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>f1-108G</v>
       </c>
     </row>
@@ -2845,7 +2851,7 @@
         <v>74</v>
       </c>
       <c r="K33" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO tblNode VALUES (32, 'f1-108A1_12', 646, 1847, 1, 'WP', 'Walk-In Clinic');</v>
       </c>
       <c r="S33" t="s">
@@ -2858,35 +2864,35 @@
         <v>28</v>
       </c>
       <c r="X33" t="str">
-        <f>$B33</f>
+        <f t="shared" si="0"/>
         <v>f1-108A1_12</v>
       </c>
       <c r="Y33" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>f1-108A1_11</v>
       </c>
       <c r="Z33" t="str">
-        <f>$B33</f>
+        <f t="shared" si="1"/>
         <v>f1-108A1_12</v>
       </c>
       <c r="AA33" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>f1-108I</v>
       </c>
       <c r="AB33" t="str">
-        <f>$B33</f>
+        <f t="shared" si="6"/>
         <v>f1-108A1_12</v>
       </c>
       <c r="AC33" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>f1-108H</v>
       </c>
       <c r="AD33" t="str">
-        <f>$B33</f>
+        <f t="shared" si="8"/>
         <v>f1-108A1_12</v>
       </c>
       <c r="AE33">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -2913,42 +2919,42 @@
         <v>82</v>
       </c>
       <c r="K34" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO tblNode VALUES (33, 'f1-108B', 834, 2634, 1, 'Exam Room', 'Walk-In Clinic');</v>
       </c>
       <c r="S34" t="s">
         <v>33</v>
       </c>
       <c r="X34" t="str">
-        <f>$B34</f>
+        <f t="shared" ref="X34:X50" si="10">$B34</f>
         <v>f1-108B</v>
       </c>
       <c r="Y34" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>f1-108A1_1</v>
       </c>
       <c r="Z34" t="str">
-        <f>$B34</f>
+        <f t="shared" ref="Z34:Z50" si="11">$B34</f>
         <v>f1-108B</v>
       </c>
       <c r="AA34">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AB34" t="str">
-        <f>$B34</f>
+        <f t="shared" si="6"/>
         <v>f1-108B</v>
       </c>
       <c r="AC34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AD34" t="str">
-        <f>$B34</f>
+        <f t="shared" si="8"/>
         <v>f1-108B</v>
       </c>
       <c r="AE34">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -2975,42 +2981,42 @@
         <v>82</v>
       </c>
       <c r="K35" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO tblNode VALUES (34, 'f1-108C', 717, 2519, 1, 'Closet', 'Walk-In Clinic');</v>
       </c>
       <c r="S35" t="s">
         <v>35</v>
       </c>
       <c r="X35" t="str">
-        <f>$B35</f>
+        <f t="shared" si="10"/>
         <v>f1-108C</v>
       </c>
       <c r="Y35" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>f1-108A1_3</v>
       </c>
       <c r="Z35" t="str">
-        <f>$B35</f>
+        <f t="shared" si="11"/>
         <v>f1-108C</v>
       </c>
       <c r="AA35">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AB35" t="str">
-        <f>$B35</f>
+        <f t="shared" si="6"/>
         <v>f1-108C</v>
       </c>
       <c r="AC35">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AD35" t="str">
-        <f>$B35</f>
+        <f t="shared" si="8"/>
         <v>f1-108C</v>
       </c>
       <c r="AE35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -3037,42 +3043,42 @@
         <v>82</v>
       </c>
       <c r="K36" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO tblNode VALUES (35, 'f1-108D', 717, 2360, 1, 'Closet', 'Walk-In Clinic');</v>
       </c>
       <c r="S36" t="s">
         <v>37</v>
       </c>
       <c r="X36" t="str">
-        <f>$B36</f>
+        <f t="shared" si="10"/>
         <v>f1-108D</v>
       </c>
       <c r="Y36" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>f1-108A1_5</v>
       </c>
       <c r="Z36" t="str">
-        <f>$B36</f>
+        <f t="shared" si="11"/>
         <v>f1-108D</v>
       </c>
       <c r="AA36">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AB36" t="str">
-        <f>$B36</f>
+        <f t="shared" si="6"/>
         <v>f1-108D</v>
       </c>
       <c r="AC36">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AD36" t="str">
-        <f>$B36</f>
+        <f t="shared" si="8"/>
         <v>f1-108D</v>
       </c>
       <c r="AE36">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -3099,42 +3105,42 @@
         <v>82</v>
       </c>
       <c r="K37" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO tblNode VALUES (36, 'f1-108E', 834, 2235, 1, 'Exam Room', 'Walk-In Clinic');</v>
       </c>
       <c r="S37" t="s">
         <v>39</v>
       </c>
       <c r="X37" t="str">
-        <f>$B37</f>
+        <f t="shared" si="10"/>
         <v>f1-108E</v>
       </c>
       <c r="Y37" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>f1-108A1_7</v>
       </c>
       <c r="Z37" t="str">
-        <f>$B37</f>
+        <f t="shared" si="11"/>
         <v>f1-108E</v>
       </c>
       <c r="AA37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AB37" t="str">
-        <f>$B37</f>
+        <f t="shared" si="6"/>
         <v>f1-108E</v>
       </c>
       <c r="AC37">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AD37" t="str">
-        <f>$B37</f>
+        <f t="shared" si="8"/>
         <v>f1-108E</v>
       </c>
       <c r="AE37">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -3161,42 +3167,42 @@
         <v>82</v>
       </c>
       <c r="K38" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO tblNode VALUES (37, 'f1-108F', 834, 2145, 1, 'Exam Room', 'Walk-In Clinic');</v>
       </c>
       <c r="S38" t="s">
         <v>41</v>
       </c>
       <c r="X38" t="str">
-        <f>$B38</f>
+        <f t="shared" si="10"/>
         <v>f1-108F</v>
       </c>
       <c r="Y38" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>f1-108A1_9</v>
       </c>
       <c r="Z38" t="str">
-        <f>$B38</f>
+        <f t="shared" si="11"/>
         <v>f1-108F</v>
       </c>
       <c r="AA38">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AB38" t="str">
-        <f>$B38</f>
+        <f t="shared" si="6"/>
         <v>f1-108F</v>
       </c>
       <c r="AC38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AD38" t="str">
-        <f>$B38</f>
+        <f t="shared" si="8"/>
         <v>f1-108F</v>
       </c>
       <c r="AE38">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -3223,42 +3229,42 @@
         <v>82</v>
       </c>
       <c r="K39" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO tblNode VALUES (38, 'f1-108G', 717, 1986, 1, 'Closet', 'Walk-In Clinic');</v>
       </c>
       <c r="S39" t="s">
         <v>43</v>
       </c>
       <c r="X39" t="str">
-        <f>$B39</f>
+        <f t="shared" si="10"/>
         <v>f1-108G</v>
       </c>
       <c r="Y39" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>f1-108A1_11</v>
       </c>
       <c r="Z39" t="str">
-        <f>$B39</f>
+        <f t="shared" si="11"/>
         <v>f1-108G</v>
       </c>
       <c r="AA39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AB39" t="str">
-        <f>$B39</f>
+        <f t="shared" si="6"/>
         <v>f1-108G</v>
       </c>
       <c r="AC39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AD39" t="str">
-        <f>$B39</f>
+        <f t="shared" si="8"/>
         <v>f1-108G</v>
       </c>
       <c r="AE39">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -3285,42 +3291,42 @@
         <v>82</v>
       </c>
       <c r="K40" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO tblNode VALUES (39, 'f1-108H', 834, 1847, 1, 'Exam Room', 'Walk-In Clinic');</v>
       </c>
       <c r="S40" t="s">
         <v>44</v>
       </c>
       <c r="X40" t="str">
-        <f>$B40</f>
+        <f t="shared" si="10"/>
         <v>f1-108H</v>
       </c>
       <c r="Y40" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>f1-108A1_12</v>
       </c>
       <c r="Z40" t="str">
-        <f>$B40</f>
+        <f t="shared" si="11"/>
         <v>f1-108H</v>
       </c>
       <c r="AA40">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AB40" t="str">
-        <f>$B40</f>
+        <f t="shared" si="6"/>
         <v>f1-108H</v>
       </c>
       <c r="AC40">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AD40" t="str">
-        <f>$B40</f>
+        <f t="shared" si="8"/>
         <v>f1-108H</v>
       </c>
       <c r="AE40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -3347,42 +3353,42 @@
         <v>82</v>
       </c>
       <c r="K41" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO tblNode VALUES (40, 'f1-108I', 460, 1847, 1, 'Exam Room', 'Walk-In Clinic');</v>
       </c>
       <c r="S41" t="s">
         <v>44</v>
       </c>
       <c r="X41" t="str">
-        <f>$B41</f>
+        <f t="shared" si="10"/>
         <v>f1-108I</v>
       </c>
       <c r="Y41" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>f1-108A1_12</v>
       </c>
       <c r="Z41" t="str">
-        <f>$B41</f>
+        <f t="shared" si="11"/>
         <v>f1-108I</v>
       </c>
       <c r="AA41">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AB41" t="str">
-        <f>$B41</f>
+        <f t="shared" si="6"/>
         <v>f1-108I</v>
       </c>
       <c r="AC41">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AD41" t="str">
-        <f>$B41</f>
+        <f t="shared" si="8"/>
         <v>f1-108I</v>
       </c>
       <c r="AE41">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -3409,42 +3415,42 @@
         <v>82</v>
       </c>
       <c r="K42" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO tblNode VALUES (41, 'f1-108J', 579, 1986, 1, 'Closet', 'Walk-In Clinic');</v>
       </c>
       <c r="S42" t="s">
         <v>43</v>
       </c>
       <c r="X42" t="str">
-        <f>$B42</f>
+        <f t="shared" si="10"/>
         <v>f1-108J</v>
       </c>
       <c r="Y42" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>f1-108A1_11</v>
       </c>
       <c r="Z42" t="str">
-        <f>$B42</f>
+        <f t="shared" si="11"/>
         <v>f1-108J</v>
       </c>
       <c r="AA42">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AB42" t="str">
-        <f>$B42</f>
+        <f t="shared" si="6"/>
         <v>f1-108J</v>
       </c>
       <c r="AC42">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AD42" t="str">
-        <f>$B42</f>
+        <f t="shared" si="8"/>
         <v>f1-108J</v>
       </c>
       <c r="AE42">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -3471,42 +3477,42 @@
         <v>82</v>
       </c>
       <c r="K43" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO tblNode VALUES (42, 'f1-108K', 460, 2100, 1, 'Exam Room', 'Walk-In Clinic');</v>
       </c>
       <c r="S43" t="s">
         <v>42</v>
       </c>
       <c r="X43" t="str">
-        <f>$B43</f>
+        <f t="shared" si="10"/>
         <v>f1-108K</v>
       </c>
       <c r="Y43" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>f1-108A1_10</v>
       </c>
       <c r="Z43" t="str">
-        <f>$B43</f>
+        <f t="shared" si="11"/>
         <v>f1-108K</v>
       </c>
       <c r="AA43">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AB43" t="str">
-        <f>$B43</f>
+        <f t="shared" si="6"/>
         <v>f1-108K</v>
       </c>
       <c r="AC43">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AD43" t="str">
-        <f>$B43</f>
+        <f t="shared" si="8"/>
         <v>f1-108K</v>
       </c>
       <c r="AE43">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -3533,42 +3539,42 @@
         <v>82</v>
       </c>
       <c r="K44" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO tblNode VALUES (43, 'f1-108L', 460, 2200, 1, 'Exam Room', 'Walk-In Clinic');</v>
       </c>
       <c r="S44" t="s">
         <v>40</v>
       </c>
       <c r="X44" t="str">
-        <f>$B44</f>
+        <f t="shared" si="10"/>
         <v>f1-108L</v>
       </c>
       <c r="Y44" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>f1-108A1_8</v>
       </c>
       <c r="Z44" t="str">
-        <f>$B44</f>
+        <f t="shared" si="11"/>
         <v>f1-108L</v>
       </c>
       <c r="AA44">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AB44" t="str">
-        <f>$B44</f>
+        <f t="shared" si="6"/>
         <v>f1-108L</v>
       </c>
       <c r="AC44">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AD44" t="str">
-        <f>$B44</f>
+        <f t="shared" si="8"/>
         <v>f1-108L</v>
       </c>
       <c r="AE44">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -3595,42 +3601,42 @@
         <v>82</v>
       </c>
       <c r="K45" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO tblNode VALUES (44, 'f1-108O', 460, 2558, 1, 'Exam Room', 'Walk-In Clinic');</v>
       </c>
       <c r="S45" t="s">
         <v>34</v>
       </c>
       <c r="X45" t="str">
-        <f>$B45</f>
+        <f t="shared" si="10"/>
         <v>f1-108O</v>
       </c>
       <c r="Y45" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>f1-108A1_2</v>
       </c>
       <c r="Z45" t="str">
-        <f>$B45</f>
+        <f t="shared" si="11"/>
         <v>f1-108O</v>
       </c>
       <c r="AA45">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AB45" t="str">
-        <f>$B45</f>
+        <f t="shared" si="6"/>
         <v>f1-108O</v>
       </c>
       <c r="AC45">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AD45" t="str">
-        <f>$B45</f>
+        <f t="shared" si="8"/>
         <v>f1-108O</v>
       </c>
       <c r="AE45">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -3657,7 +3663,7 @@
         <v>82</v>
       </c>
       <c r="K46" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO tblNode VALUES (45, 'f1-108P', 460, 2738, 1, 'Exam Room', 'Walk-In Clinic');</v>
       </c>
       <c r="S46" t="s">
@@ -3667,35 +3673,35 @@
         <v>50</v>
       </c>
       <c r="X46" t="str">
-        <f>$B46</f>
+        <f t="shared" si="10"/>
         <v>f1-108P</v>
       </c>
       <c r="Y46" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>f1-108A1_0</v>
       </c>
       <c r="Z46" t="str">
-        <f>$B46</f>
+        <f t="shared" si="11"/>
         <v>f1-108P</v>
       </c>
       <c r="AA46" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>f1-108P_0</v>
       </c>
       <c r="AB46" t="str">
-        <f>$B46</f>
+        <f t="shared" si="6"/>
         <v>f1-108P</v>
       </c>
       <c r="AC46">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AD46" t="str">
-        <f>$B46</f>
+        <f t="shared" si="8"/>
         <v>f1-108P</v>
       </c>
       <c r="AE46">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -3722,7 +3728,7 @@
         <v>82</v>
       </c>
       <c r="K47" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO tblNode VALUES (46, 'f1-108P_0', 227, 2738, 1, 'WP', 'Walk-In Clinic');</v>
       </c>
       <c r="S47" t="s">
@@ -3732,35 +3738,35 @@
         <v>49</v>
       </c>
       <c r="X47" t="str">
-        <f>$B47</f>
+        <f t="shared" si="10"/>
         <v>f1-108P_0</v>
       </c>
       <c r="Y47" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>f1-108P</v>
       </c>
       <c r="Z47" t="str">
-        <f>$B47</f>
+        <f t="shared" si="11"/>
         <v>f1-108P_0</v>
       </c>
       <c r="AA47" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>f1-108Q</v>
       </c>
       <c r="AB47" t="str">
-        <f>$B47</f>
+        <f t="shared" si="6"/>
         <v>f1-108P_0</v>
       </c>
       <c r="AC47">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AD47" t="str">
-        <f>$B47</f>
+        <f t="shared" si="8"/>
         <v>f1-108P_0</v>
       </c>
       <c r="AE47">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -3787,42 +3793,42 @@
         <v>82</v>
       </c>
       <c r="K48" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO tblNode VALUES (47, 'f1-108Q', 227, 3005, 1, 'Exam Room', 'Walk-In Clinic');</v>
       </c>
       <c r="S48" t="s">
         <v>50</v>
       </c>
       <c r="X48" t="str">
-        <f>$B48</f>
+        <f t="shared" si="10"/>
         <v>f1-108Q</v>
       </c>
       <c r="Y48" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>f1-108P_0</v>
       </c>
       <c r="Z48" t="str">
-        <f>$B48</f>
+        <f t="shared" si="11"/>
         <v>f1-108Q</v>
       </c>
       <c r="AA48">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AB48" t="str">
-        <f>$B48</f>
+        <f t="shared" si="6"/>
         <v>f1-108Q</v>
       </c>
       <c r="AC48">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AD48" t="str">
-        <f>$B48</f>
+        <f t="shared" si="8"/>
         <v>f1-108Q</v>
       </c>
       <c r="AE48">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -3852,42 +3858,42 @@
         <v>71</v>
       </c>
       <c r="K49" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO tblNode VALUES (48, 'f1-108T1', 579, 2281, 1, 'Restroom', 'Walk-In Clinic');</v>
       </c>
       <c r="S49" t="s">
         <v>36</v>
       </c>
       <c r="X49" t="str">
-        <f>$B49</f>
+        <f t="shared" si="10"/>
         <v>f1-108T1</v>
       </c>
       <c r="Y49" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>f1-108A1_4</v>
       </c>
       <c r="Z49" t="str">
-        <f>$B49</f>
+        <f t="shared" si="11"/>
         <v>f1-108T1</v>
       </c>
       <c r="AA49">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AB49" t="str">
-        <f>$B49</f>
+        <f t="shared" si="6"/>
         <v>f1-108T1</v>
       </c>
       <c r="AC49">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AD49" t="str">
-        <f>$B49</f>
+        <f t="shared" si="8"/>
         <v>f1-108T1</v>
       </c>
       <c r="AE49">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -3917,42 +3923,42 @@
         <v>71</v>
       </c>
       <c r="K50" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO tblNode VALUES (49, 'f1-108T2', 579, 2477, 1, 'Restroom', 'Walk-In Clinic');</v>
       </c>
       <c r="S50" t="s">
         <v>38</v>
       </c>
       <c r="X50" t="str">
-        <f>$B50</f>
+        <f t="shared" si="10"/>
         <v>f1-108T2</v>
       </c>
       <c r="Y50" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>f1-108A1_6</v>
       </c>
       <c r="Z50" t="str">
-        <f>$B50</f>
+        <f t="shared" si="11"/>
         <v>f1-108T2</v>
       </c>
       <c r="AA50">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AB50" t="str">
-        <f>$B50</f>
+        <f t="shared" si="6"/>
         <v>f1-108T2</v>
       </c>
       <c r="AC50">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AD50" t="str">
-        <f>$B50</f>
+        <f t="shared" si="8"/>
         <v>f1-108T2</v>
       </c>
       <c r="AE50">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -3969,10 +3975,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F95"/>
+  <dimension ref="A1:F100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4020,7 +4026,7 @@
         <v>54</v>
       </c>
       <c r="F3" t="str">
-        <f t="shared" ref="F3:F66" si="0">E$1 &amp; A3 &amp; ", '" &amp; B3 &amp; "', '" &amp; C3 &amp; "');"</f>
+        <f t="shared" ref="F3:F63" si="0">E$1 &amp; A3 &amp; ", '" &amp; B3 &amp; "', '" &amp; C3 &amp; "');"</f>
         <v>INSERT INTO tblNeighbors VALUES (2, 'f1-nel', 'f1-100C1_0');</v>
       </c>
     </row>
@@ -4734,14 +4740,14 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C51" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="F51" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO tblNeighbors VALUES (50, 'f1-100C1_0', 'f1-nel');</v>
+        <v>INSERT INTO tblNeighbors VALUES (50, 'f1-100C1_1', 'f1-100C1_2');</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -4749,14 +4755,14 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C52" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="F52" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO tblNeighbors VALUES (51, 'f1-100C1_1', 'f1-100s3');</v>
+        <v>INSERT INTO tblNeighbors VALUES (51, 'f1-100C1_2', 'f1-100C1_3');</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -4764,14 +4770,14 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C53" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="F53" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO tblNeighbors VALUES (52, 'f1-100C1_5', 'f1-108');</v>
+        <v>INSERT INTO tblNeighbors VALUES (52, 'f1-100C1_3', 'f1-100C1_4');</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -4779,14 +4785,14 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C54" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F54" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO tblNeighbors VALUES (53, 'f1-100C2_0', 'f1-sel');</v>
+        <v>INSERT INTO tblNeighbors VALUES (53, 'f1-100C1_4', 'f1-100C1_5');</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -4794,14 +4800,14 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C55" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F55" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO tblNeighbors VALUES (54, 'f1-100C3_1', 'f1-100s2');</v>
+        <v>INSERT INTO tblNeighbors VALUES (54, 'f1-100C1_5', 'f1-100C2_0');</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -4809,14 +4815,14 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>32</v>
+        <v>62</v>
       </c>
       <c r="C56" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="F56" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO tblNeighbors VALUES (55, 'f1-108A1_0', 'f1-108P');</v>
+        <v>INSERT INTO tblNeighbors VALUES (55, 'f1-100C2_0', 'f1-100C3_0');</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
@@ -4824,14 +4830,14 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="C57" t="s">
-        <v>22</v>
+        <v>63</v>
       </c>
       <c r="F57" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO tblNeighbors VALUES (56, 'f1-108A1_1', 'f1-108B');</v>
+        <v>INSERT INTO tblNeighbors VALUES (56, 'f1-100C3_0', 'f1-100C3_1');</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -4839,14 +4845,14 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>34</v>
+        <v>63</v>
       </c>
       <c r="C58" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="F58" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO tblNeighbors VALUES (57, 'f1-108A1_2', 'f1-108O');</v>
+        <v>INSERT INTO tblNeighbors VALUES (57, 'f1-100C3_1', 'f1-100C3_1');</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -4854,14 +4860,14 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="C59" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="F59" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO tblNeighbors VALUES (58, 'f1-108A1_3', 'f1-108C');</v>
+        <v>INSERT INTO tblNeighbors VALUES (58, 'f1-108', 'f1-108_0');</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -4869,14 +4875,14 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="C60" t="s">
-        <v>65</v>
+        <v>14</v>
       </c>
       <c r="F60" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO tblNeighbors VALUES (59, 'f1-108A1_4', 'f1-108T1');</v>
+        <v>INSERT INTO tblNeighbors VALUES (59, 'f1-108_0', 'f1-108_1');</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
@@ -4884,14 +4890,14 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="C61" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="F61" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO tblNeighbors VALUES (60, 'f1-108A1_5', 'f1-108D');</v>
+        <v>INSERT INTO tblNeighbors VALUES (60, 'f1-108_1', 'f1-108_2');</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
@@ -4899,14 +4905,14 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="C62" t="s">
-        <v>66</v>
+        <v>14</v>
       </c>
       <c r="F62" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO tblNeighbors VALUES (61, 'f1-108A1_6', 'f1-108T2');</v>
+        <v>INSERT INTO tblNeighbors VALUES (61, 'f1-108_2', 'f1-108_1');</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
@@ -4914,14 +4920,14 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="C63" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="F63" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO tblNeighbors VALUES (62, 'f1-108A1_7', 'f1-108E');</v>
+        <v>INSERT INTO tblNeighbors VALUES (62, 'f1-108A1', 'f1-108_2');</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -4929,14 +4935,14 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="C64" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="F64" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO tblNeighbors VALUES (63, 'f1-108A1_8', 'f1-108L');</v>
+        <f t="shared" ref="F64:F100" si="1">E$1 &amp; A64 &amp; ", '" &amp; B64 &amp; "', '" &amp; C64 &amp; "');"</f>
+        <v>INSERT INTO tblNeighbors VALUES (63, 'f1-108A1_0', 'f1-108A1_1');</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -4944,14 +4950,14 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C65" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="F65" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO tblNeighbors VALUES (64, 'f1-108A1_9', 'f1-108F');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO tblNeighbors VALUES (64, 'f1-108A1_1', 'f1-108A1_2');</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -4959,14 +4965,14 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="C66" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="F66" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO tblNeighbors VALUES (65, 'f1-108A1_10', 'f1-108K');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO tblNeighbors VALUES (65, 'f1-108A1_2', 'f1-108A1_3');</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -4974,14 +4980,14 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="C67" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="F67" t="str">
-        <f t="shared" ref="F67:F95" si="1">E$1 &amp; A67 &amp; ", '" &amp; B67 &amp; "', '" &amp; C67 &amp; "');"</f>
-        <v>INSERT INTO tblNeighbors VALUES (66, 'f1-108A1_11', 'f1-108J');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO tblNeighbors VALUES (66, 'f1-108A1_3', 'f1-108A1_4');</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -4989,14 +4995,14 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="C68" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="F68" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tblNeighbors VALUES (67, 'f1-108A1_12', 'f1-108H');</v>
+        <v>INSERT INTO tblNeighbors VALUES (67, 'f1-108A1_4', 'f1-108A1_5');</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -5004,14 +5010,14 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C69" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="F69" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tblNeighbors VALUES (68, 'f1-108A1_11', 'f1-108G');</v>
+        <v>INSERT INTO tblNeighbors VALUES (68, 'f1-108A1_5', 'f1-108A1_6');</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -5019,14 +5025,14 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="C70" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="F70" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tblNeighbors VALUES (69, 'f1-100C1_1', 'f1-100C1_2');</v>
+        <v>INSERT INTO tblNeighbors VALUES (69, 'f1-108A1_6', 'f1-108A1_7');</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
@@ -5034,14 +5040,14 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="C71" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="F71" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tblNeighbors VALUES (70, 'f1-100C1_2', 'f1-100C1_3');</v>
+        <v>INSERT INTO tblNeighbors VALUES (70, 'f1-108A1_7', 'f1-108A1_8');</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
@@ -5049,14 +5055,14 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="C72" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="F72" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tblNeighbors VALUES (71, 'f1-100C1_3', 'f1-100C1_4');</v>
+        <v>INSERT INTO tblNeighbors VALUES (71, 'f1-108A1_8', 'f1-108A1_9');</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
@@ -5064,14 +5070,14 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="C73" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="F73" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tblNeighbors VALUES (72, 'f1-100C1_4', 'f1-100C1_5');</v>
+        <v>INSERT INTO tblNeighbors VALUES (72, 'f1-108A1_9', 'f1-108A1_10');</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
@@ -5079,14 +5085,14 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="C74" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="F74" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tblNeighbors VALUES (73, 'f1-100C1_5', 'f1-100C2_0');</v>
+        <v>INSERT INTO tblNeighbors VALUES (73, 'f1-108A1_10', 'f1-108A1_11');</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
@@ -5094,14 +5100,14 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="C75" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="F75" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tblNeighbors VALUES (74, 'f1-100C2_0', 'f1-100C3_0');</v>
+        <v>INSERT INTO tblNeighbors VALUES (74, 'f1-108A1_11', 'f1-108A1_12');</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
@@ -5109,14 +5115,14 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C76" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="F76" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tblNeighbors VALUES (75, 'f1-108', 'f1-108_0');</v>
+        <v>INSERT INTO tblNeighbors VALUES (75, 'f1-108A1_12', 'f1-108I');</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
@@ -5124,14 +5130,14 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="C77" t="s">
-        <v>14</v>
+        <v>50</v>
       </c>
       <c r="F77" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tblNeighbors VALUES (76, 'f1-108_0', 'f1-108_1');</v>
+        <v>INSERT INTO tblNeighbors VALUES (76, 'f1-108P', 'f1-108P_0');</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
@@ -5139,14 +5145,14 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>14</v>
+        <v>50</v>
       </c>
       <c r="C78" t="s">
-        <v>15</v>
+        <v>49</v>
       </c>
       <c r="F78" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tblNeighbors VALUES (77, 'f1-108_1', 'f1-108_2');</v>
+        <v>INSERT INTO tblNeighbors VALUES (77, 'f1-108P_0', 'f1-108Q');</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
@@ -5154,14 +5160,14 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="C79" t="s">
-        <v>14</v>
+        <v>50</v>
       </c>
       <c r="F79" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tblNeighbors VALUES (78, 'f1-108_2', 'f1-108_1');</v>
+        <v>INSERT INTO tblNeighbors VALUES (78, 'f1-108P', 'f1-108P_0');</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
@@ -5169,14 +5175,14 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C80" t="s">
-        <v>15</v>
+        <v>49</v>
       </c>
       <c r="F80" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tblNeighbors VALUES (79, 'f1-108A1', 'f1-108_2');</v>
+        <v>INSERT INTO tblNeighbors VALUES (79, 'f1-108P_0', 'f1-108Q');</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
@@ -5184,14 +5190,14 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="C81" t="s">
-        <v>33</v>
+        <v>60</v>
       </c>
       <c r="F81" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tblNeighbors VALUES (80, 'f1-108A1_0', 'f1-108A1_1');</v>
+        <v>INSERT INTO tblNeighbors VALUES (80, 'f1-100C1_0', 'f1-nel');</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
@@ -5199,14 +5205,14 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="C82" t="s">
-        <v>34</v>
+        <v>76</v>
       </c>
       <c r="F82" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tblNeighbors VALUES (81, 'f1-108A1_1', 'f1-108A1_2');</v>
+        <v>INSERT INTO tblNeighbors VALUES (81, 'f1-100C1_1', 'f1-100s3');</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
@@ -5214,14 +5220,14 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="C83" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="F83" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tblNeighbors VALUES (82, 'f1-108A1_2', 'f1-108A1_3');</v>
+        <v>INSERT INTO tblNeighbors VALUES (82, 'f1-100C1_3', 'f1-nr');</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
@@ -5229,14 +5235,14 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="C84" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="F84" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tblNeighbors VALUES (83, 'f1-108A1_3', 'f1-108A1_4');</v>
+        <v>INSERT INTO tblNeighbors VALUES (83, 'f1-100C1_5', 'f1-108');</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
@@ -5244,14 +5250,14 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>36</v>
+        <v>62</v>
       </c>
       <c r="C85" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="F85" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tblNeighbors VALUES (84, 'f1-108A1_4', 'f1-108A1_5');</v>
+        <v>INSERT INTO tblNeighbors VALUES (84, 'f1-100C2_0', 'f1-sel');</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
@@ -5259,14 +5265,14 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>37</v>
+        <v>63</v>
       </c>
       <c r="C86" t="s">
-        <v>38</v>
+        <v>61</v>
       </c>
       <c r="F86" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tblNeighbors VALUES (85, 'f1-108A1_5', 'f1-108A1_6');</v>
+        <v>INSERT INTO tblNeighbors VALUES (85, 'f1-100C3_1', 'f1-100s2');</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
@@ -5274,14 +5280,14 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C87" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="F87" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tblNeighbors VALUES (86, 'f1-108A1_6', 'f1-108A1_7');</v>
+        <v>INSERT INTO tblNeighbors VALUES (86, 'f1-108A1_0', 'f1-108P');</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
@@ -5289,14 +5295,14 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C88" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="F88" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tblNeighbors VALUES (87, 'f1-108A1_7', 'f1-108A1_8');</v>
+        <v>INSERT INTO tblNeighbors VALUES (87, 'f1-108A1_1', 'f1-108B');</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
@@ -5304,14 +5310,14 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C89" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="F89" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tblNeighbors VALUES (88, 'f1-108A1_8', 'f1-108A1_9');</v>
+        <v>INSERT INTO tblNeighbors VALUES (88, 'f1-108A1_2', 'f1-108O');</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
@@ -5319,14 +5325,14 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C90" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="F90" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tblNeighbors VALUES (89, 'f1-108A1_9', 'f1-108A1_10');</v>
+        <v>INSERT INTO tblNeighbors VALUES (89, 'f1-108A1_3', 'f1-108C');</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
@@ -5334,14 +5340,14 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C91" t="s">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="F91" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tblNeighbors VALUES (90, 'f1-108A1_10', 'f1-108A1_11');</v>
+        <v>INSERT INTO tblNeighbors VALUES (90, 'f1-108A1_4', 'f1-108T1');</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
@@ -5349,14 +5355,14 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C92" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="F92" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tblNeighbors VALUES (91, 'f1-108A1_11', 'f1-108A1_12');</v>
+        <v>INSERT INTO tblNeighbors VALUES (91, 'f1-108A1_5', 'f1-108D');</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
@@ -5364,14 +5370,14 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C93" t="s">
-        <v>29</v>
+        <v>66</v>
       </c>
       <c r="F93" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tblNeighbors VALUES (92, 'f1-108A1_12', 'f1-108I');</v>
+        <v>INSERT INTO tblNeighbors VALUES (92, 'f1-108A1_6', 'f1-108T2');</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
@@ -5379,14 +5385,14 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="C94" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="F94" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tblNeighbors VALUES (93, 'f1-108P', 'f1-108P_0');</v>
+        <v>INSERT INTO tblNeighbors VALUES (93, 'f1-108A1_7', 'f1-108E');</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
@@ -5394,14 +5400,89 @@
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C95" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F95" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO tblNeighbors VALUES (94, 'f1-108P_0', 'f1-108Q');</v>
+        <v>INSERT INTO tblNeighbors VALUES (94, 'f1-108A1_8', 'f1-108L');</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>95</v>
+      </c>
+      <c r="B96" t="s">
+        <v>41</v>
+      </c>
+      <c r="C96" t="s">
+        <v>26</v>
+      </c>
+      <c r="F96" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO tblNeighbors VALUES (95, 'f1-108A1_9', 'f1-108F');</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>96</v>
+      </c>
+      <c r="B97" t="s">
+        <v>42</v>
+      </c>
+      <c r="C97" t="s">
+        <v>31</v>
+      </c>
+      <c r="F97" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO tblNeighbors VALUES (96, 'f1-108A1_10', 'f1-108K');</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>97</v>
+      </c>
+      <c r="B98" t="s">
+        <v>43</v>
+      </c>
+      <c r="C98" t="s">
+        <v>30</v>
+      </c>
+      <c r="F98" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO tblNeighbors VALUES (97, 'f1-108A1_11', 'f1-108J');</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>98</v>
+      </c>
+      <c r="B99" t="s">
+        <v>44</v>
+      </c>
+      <c r="C99" t="s">
+        <v>28</v>
+      </c>
+      <c r="F99" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO tblNeighbors VALUES (98, 'f1-108A1_12', 'f1-108H');</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>99</v>
+      </c>
+      <c r="B100" t="s">
+        <v>43</v>
+      </c>
+      <c r="C100" t="s">
+        <v>27</v>
+      </c>
+      <c r="F100" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO tblNeighbors VALUES (99, 'f1-108A1_11', 'f1-108G');</v>
       </c>
     </row>
   </sheetData>

</xml_diff>